<commit_message>
state of the art
</commit_message>
<xml_diff>
--- a/PROJEK AKHIR KITA SEBELUM UTS/4State of The Art.xlsx
+++ b/PROJEK AKHIR KITA SEBELUM UTS/4State of The Art.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah 6\ProjekBersama\PROJEK AKHIR KITA SEBELUM UTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495294EB-4FC0-4F72-956F-ECF5E990F672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37411872-1F1D-41DD-8549-FF21823253E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7995" xr2:uid="{EEE36F96-FF2A-466B-BBC3-0DC5B31D1F19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{EEE36F96-FF2A-466B-BBC3-0DC5B31D1F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1543,11 +1543,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB84D94A-7B16-4F43-B3F4-B11B622CF43E}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1365" ySplit="630" topLeftCell="A12" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1110"/>
+      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="405" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="344.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1721,7 +1720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="312.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="276" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="319.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="334.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>12</v>
       </c>

</xml_diff>